<commit_message>
Finished the report. All the figures exported to ps and then gone to eps. under the section of evaluation there is a table out of place. todo!
</commit_message>
<xml_diff>
--- a/Reports/Phase C/evaluation.xlsx
+++ b/Reports/Phase C/evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="744" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="826" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -309,11 +309,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124439720"/>
-        <c:axId val="2124432856"/>
+        <c:axId val="2054171912"/>
+        <c:axId val="2054165048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2124439720"/>
+        <c:axId val="2054171912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -349,7 +349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124432856"/>
+        <c:crossAx val="2054165048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -357,7 +357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124432856"/>
+        <c:axId val="2054165048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,7 +394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124439720"/>
+        <c:crossAx val="2054171912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -513,11 +513,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126021480"/>
-        <c:axId val="2126027000"/>
+        <c:axId val="2101920920"/>
+        <c:axId val="2101926440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126021480"/>
+        <c:axId val="2101920920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126027000"/>
+        <c:crossAx val="2101926440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -561,7 +561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126027000"/>
+        <c:axId val="2101926440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126021480"/>
+        <c:crossAx val="2101920920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,11 +722,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126060008"/>
-        <c:axId val="2126065752"/>
+        <c:axId val="2101959800"/>
+        <c:axId val="2101965544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126060008"/>
+        <c:axId val="2101959800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126065752"/>
+        <c:crossAx val="2101965544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -775,7 +775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126065752"/>
+        <c:axId val="2101965544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -817,7 +817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126060008"/>
+        <c:crossAx val="2101959800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,11 +998,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2116150440"/>
-        <c:axId val="-2116148680"/>
+        <c:axId val="2102002088"/>
+        <c:axId val="2102007576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2116150440"/>
+        <c:axId val="2102002088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1038,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116148680"/>
+        <c:crossAx val="2102007576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1046,7 +1046,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116148680"/>
+        <c:axId val="2102007576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116150440"/>
+        <c:crossAx val="2102002088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1196,11 +1196,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2135713032"/>
-        <c:axId val="2135578104"/>
+        <c:axId val="2102053064"/>
+        <c:axId val="2102058776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2135713032"/>
+        <c:axId val="2102053064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135578104"/>
+        <c:crossAx val="2102058776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1249,7 +1249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135578104"/>
+        <c:axId val="2102058776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135713032"/>
+        <c:crossAx val="2102053064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1395,11 +1395,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115409192"/>
-        <c:axId val="-2115403496"/>
+        <c:axId val="2102101240"/>
+        <c:axId val="2102106952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115409192"/>
+        <c:axId val="2102101240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115403496"/>
+        <c:crossAx val="2102106952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1448,7 +1448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115403496"/>
+        <c:axId val="2102106952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115409192"/>
+        <c:crossAx val="2102101240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1594,11 +1594,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139030968"/>
-        <c:axId val="2139036664"/>
+        <c:axId val="2102149448"/>
+        <c:axId val="2102154904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139030968"/>
+        <c:axId val="2102149448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139036664"/>
+        <c:crossAx val="2102154904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1642,7 +1642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139036664"/>
+        <c:axId val="2102154904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,7 +1679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139030968"/>
+        <c:crossAx val="2102149448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1788,11 +1788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115130504"/>
-        <c:axId val="-2115152104"/>
+        <c:axId val="2102197496"/>
+        <c:axId val="2102202936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115130504"/>
+        <c:axId val="2102197496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,7 +1828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115152104"/>
+        <c:crossAx val="2102202936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1836,7 +1836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115152104"/>
+        <c:axId val="2102202936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115130504"/>
+        <c:crossAx val="2102197496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -3623,8 +3623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3760,12 +3760,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3780,12 +3782,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -12986,6 +12990,7 @@
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
@@ -13013,6 +13018,7 @@
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
@@ -13040,6 +13046,7 @@
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
@@ -13064,7 +13071,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -13084,7 +13093,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>